<commit_message>
Refactored markers to use worksheets Added setup.cfg
</commit_message>
<xml_diff>
--- a/tests/testfiles/Test1.xlsx
+++ b/tests/testfiles/Test1.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dateien\Programmieren\PyCharm\xcelios\tests\testfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F9A5AD-279E-4C6E-B14E-B4CF21C76626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD94F0C-F60D-4B05-BF9F-ECB2A9E7ACC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5235" yWindow="330" windowWidth="21390" windowHeight="13275" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22560" yWindow="4905" windowWidth="21390" windowHeight="13275" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="SheetE" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="table_people">Sheet1!$B$3</definedName>
@@ -629,11 +630,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:Q27"/>
+  <dimension ref="B3:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1052,168 +1051,168 @@
         <v>43845</v>
       </c>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>75</v>
-      </c>
-      <c r="C25">
-        <v>87.87</v>
-      </c>
-      <c r="D25" s="3">
-        <v>148.78</v>
-      </c>
-      <c r="E25" s="3">
-        <v>146</v>
-      </c>
-      <c r="F25" s="3">
-        <v>122.82</v>
-      </c>
-      <c r="G25" s="3">
-        <v>59.77</v>
-      </c>
-      <c r="H25" s="3">
-        <v>185.34</v>
-      </c>
-      <c r="I25" s="3">
-        <v>161.47</v>
-      </c>
-      <c r="J25" s="3">
-        <v>102.02</v>
-      </c>
-      <c r="K25" s="3">
-        <v>159.44999999999999</v>
-      </c>
-      <c r="L25" s="3">
-        <v>141.33000000000001</v>
-      </c>
-      <c r="M25" s="3">
-        <v>56.67</v>
-      </c>
-      <c r="N25" s="3">
-        <v>103.83</v>
-      </c>
-      <c r="O25" s="3">
-        <v>153.31</v>
-      </c>
-      <c r="P25" s="3">
-        <v>143.16999999999999</v>
-      </c>
-      <c r="Q25" s="3">
-        <v>56.2</v>
-      </c>
-    </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C26">
-        <v>135.18</v>
+        <v>87.87</v>
       </c>
       <c r="D26" s="3">
-        <v>117.32</v>
+        <v>148.78</v>
       </c>
       <c r="E26" s="3">
-        <v>118.39</v>
+        <v>146</v>
       </c>
       <c r="F26" s="3">
-        <v>134.72999999999999</v>
+        <v>122.82</v>
       </c>
       <c r="G26" s="3">
-        <v>70.069999999999993</v>
+        <v>59.77</v>
       </c>
       <c r="H26" s="3">
-        <v>90.45</v>
+        <v>185.34</v>
       </c>
       <c r="I26" s="3">
-        <v>114.41</v>
+        <v>161.47</v>
       </c>
       <c r="J26" s="3">
-        <v>106.34</v>
+        <v>102.02</v>
       </c>
       <c r="K26" s="3">
-        <v>146</v>
+        <v>159.44999999999999</v>
       </c>
       <c r="L26" s="3">
-        <v>118.09</v>
+        <v>141.33000000000001</v>
       </c>
       <c r="M26" s="3">
-        <v>76.72</v>
+        <v>56.67</v>
       </c>
       <c r="N26" s="3">
-        <v>68.98</v>
+        <v>103.83</v>
       </c>
       <c r="O26" s="3">
-        <v>118.72</v>
+        <v>153.31</v>
       </c>
       <c r="P26" s="3">
-        <v>117.26</v>
+        <v>143.16999999999999</v>
       </c>
       <c r="Q26" s="3">
-        <v>58.81</v>
+        <v>56.2</v>
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27">
+        <v>135.18</v>
+      </c>
+      <c r="D27" s="3">
+        <v>117.32</v>
+      </c>
+      <c r="E27" s="3">
+        <v>118.39</v>
+      </c>
+      <c r="F27" s="3">
+        <v>134.72999999999999</v>
+      </c>
+      <c r="G27" s="3">
+        <v>70.069999999999993</v>
+      </c>
+      <c r="H27" s="3">
+        <v>90.45</v>
+      </c>
+      <c r="I27" s="3">
+        <v>114.41</v>
+      </c>
+      <c r="J27" s="3">
+        <v>106.34</v>
+      </c>
+      <c r="K27" s="3">
+        <v>146</v>
+      </c>
+      <c r="L27" s="3">
+        <v>118.09</v>
+      </c>
+      <c r="M27" s="3">
+        <v>76.72</v>
+      </c>
+      <c r="N27" s="3">
+        <v>68.98</v>
+      </c>
+      <c r="O27" s="3">
+        <v>118.72</v>
+      </c>
+      <c r="P27" s="3">
+        <v>117.26</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>58.81</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>77</v>
       </c>
-      <c r="C27">
-        <f t="shared" ref="C27:Q27" si="0">SUM(C25:C26)</f>
+      <c r="C28">
+        <f>SUM(C26:C27)</f>
         <v>223.05</v>
       </c>
-      <c r="D27">
-        <f t="shared" si="0"/>
+      <c r="D28">
+        <f>SUM(D26:D27)</f>
         <v>266.10000000000002</v>
       </c>
-      <c r="E27">
-        <f t="shared" si="0"/>
+      <c r="E28">
+        <f>SUM(E26:E27)</f>
         <v>264.39</v>
       </c>
-      <c r="F27">
-        <f t="shared" si="0"/>
+      <c r="F28">
+        <f>SUM(F26:F27)</f>
         <v>257.54999999999995</v>
       </c>
-      <c r="G27">
-        <f t="shared" si="0"/>
+      <c r="G28">
+        <f>SUM(G26:G27)</f>
         <v>129.84</v>
       </c>
-      <c r="H27">
-        <f t="shared" si="0"/>
+      <c r="H28">
+        <f>SUM(H26:H27)</f>
         <v>275.79000000000002</v>
       </c>
-      <c r="I27">
-        <f t="shared" si="0"/>
+      <c r="I28">
+        <f>SUM(I26:I27)</f>
         <v>275.88</v>
       </c>
-      <c r="J27">
-        <f t="shared" si="0"/>
+      <c r="J28">
+        <f>SUM(J26:J27)</f>
         <v>208.36</v>
       </c>
-      <c r="K27">
-        <f t="shared" si="0"/>
+      <c r="K28">
+        <f>SUM(K26:K27)</f>
         <v>305.45</v>
       </c>
-      <c r="L27">
-        <f t="shared" si="0"/>
+      <c r="L28">
+        <f>SUM(L26:L27)</f>
         <v>259.42</v>
       </c>
-      <c r="M27">
-        <f t="shared" si="0"/>
+      <c r="M28">
+        <f>SUM(M26:M27)</f>
         <v>133.38999999999999</v>
       </c>
-      <c r="N27">
-        <f t="shared" si="0"/>
+      <c r="N28">
+        <f>SUM(N26:N27)</f>
         <v>172.81</v>
       </c>
-      <c r="O27">
-        <f t="shared" si="0"/>
+      <c r="O28">
+        <f>SUM(O26:O27)</f>
         <v>272.02999999999997</v>
       </c>
-      <c r="P27">
-        <f t="shared" si="0"/>
+      <c r="P28">
+        <f>SUM(P26:P27)</f>
         <v>260.43</v>
       </c>
-      <c r="Q27">
-        <f t="shared" si="0"/>
+      <c r="Q28">
+        <f>SUM(Q26:Q27)</f>
         <v>115.01</v>
       </c>
     </row>
@@ -1225,4 +1224,16 @@
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA42575C-1408-4827-B59A-7A3D15E02F5F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added write_datasets added additional position helpers (Axis) updated README
</commit_message>
<xml_diff>
--- a/tests/testfiles/Test1.xlsx
+++ b/tests/testfiles/Test1.xlsx
@@ -8,16 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dateien\Programmieren\PyCharm\xcelios\tests\testfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD94F0C-F60D-4B05-BF9F-ECB2A9E7ACC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9945B9B2-6DCC-4F15-962F-CEE82623AE5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22560" yWindow="4905" windowWidth="21390" windowHeight="13275" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12015" yWindow="1200" windowWidth="21390" windowHeight="13275" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="SheetE" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="SheetE" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="table_people" localSheetId="1">Sheet2!$B$3</definedName>
     <definedName name="table_people">Sheet1!$B$3</definedName>
+    <definedName name="table_prices" localSheetId="1">Sheet2!$B$24</definedName>
     <definedName name="table_prices">Sheet1!$B$24</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="80">
   <si>
     <t>First name</t>
   </si>
@@ -273,6 +276,12 @@
   </si>
   <si>
     <t>Sum</t>
+  </si>
+  <si>
+    <t>Hello World</t>
+  </si>
+  <si>
+    <t>this is me ;-)</t>
   </si>
 </sst>
 </file>
@@ -632,7 +641,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1156,63 +1167,63 @@
         <v>77</v>
       </c>
       <c r="C28">
-        <f>SUM(C26:C27)</f>
+        <f t="shared" ref="C28:Q28" si="0">SUM(C26:C27)</f>
         <v>223.05</v>
       </c>
       <c r="D28">
-        <f>SUM(D26:D27)</f>
+        <f t="shared" si="0"/>
         <v>266.10000000000002</v>
       </c>
       <c r="E28">
-        <f>SUM(E26:E27)</f>
+        <f t="shared" si="0"/>
         <v>264.39</v>
       </c>
       <c r="F28">
-        <f>SUM(F26:F27)</f>
+        <f t="shared" si="0"/>
         <v>257.54999999999995</v>
       </c>
       <c r="G28">
-        <f>SUM(G26:G27)</f>
+        <f t="shared" si="0"/>
         <v>129.84</v>
       </c>
       <c r="H28">
-        <f>SUM(H26:H27)</f>
+        <f t="shared" si="0"/>
         <v>275.79000000000002</v>
       </c>
       <c r="I28">
-        <f>SUM(I26:I27)</f>
+        <f t="shared" si="0"/>
         <v>275.88</v>
       </c>
       <c r="J28">
-        <f>SUM(J26:J27)</f>
+        <f t="shared" si="0"/>
         <v>208.36</v>
       </c>
       <c r="K28">
-        <f>SUM(K26:K27)</f>
+        <f t="shared" si="0"/>
         <v>305.45</v>
       </c>
       <c r="L28">
-        <f>SUM(L26:L27)</f>
+        <f t="shared" si="0"/>
         <v>259.42</v>
       </c>
       <c r="M28">
-        <f>SUM(M26:M27)</f>
+        <f t="shared" si="0"/>
         <v>133.38999999999999</v>
       </c>
       <c r="N28">
-        <f>SUM(N26:N27)</f>
+        <f t="shared" si="0"/>
         <v>172.81</v>
       </c>
       <c r="O28">
-        <f>SUM(O26:O27)</f>
+        <f t="shared" si="0"/>
         <v>272.02999999999997</v>
       </c>
       <c r="P28">
-        <f>SUM(P26:P27)</f>
+        <f t="shared" si="0"/>
         <v>260.43</v>
       </c>
       <c r="Q28">
-        <f>SUM(Q26:Q27)</f>
+        <f t="shared" si="0"/>
         <v>115.01</v>
       </c>
     </row>
@@ -1227,6 +1238,612 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCD5CC15-F7FF-415F-A394-B1D65CB160A4}">
+  <dimension ref="B3:Q28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" customWidth="1"/>
+    <col min="7" max="7" width="26" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="4">
+        <v>32320</v>
+      </c>
+      <c r="F4" s="1">
+        <v>165</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="4">
+        <v>32422</v>
+      </c>
+      <c r="F5" s="1">
+        <v>185</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="4">
+        <v>33651</v>
+      </c>
+      <c r="F6" s="1">
+        <v>151</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="4">
+        <v>35367</v>
+      </c>
+      <c r="F7" s="1">
+        <v>190</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="4">
+        <v>31396</v>
+      </c>
+      <c r="F8" s="1">
+        <v>153</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="4">
+        <v>29975</v>
+      </c>
+      <c r="F9" s="1">
+        <v>174</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="4">
+        <v>35043</v>
+      </c>
+      <c r="F10" s="1">
+        <v>157</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="4">
+        <v>33040</v>
+      </c>
+      <c r="F11" s="1">
+        <v>192</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="4">
+        <v>30340</v>
+      </c>
+      <c r="F12" s="1">
+        <v>187</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="4">
+        <v>28276</v>
+      </c>
+      <c r="F13" s="1">
+        <v>160</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="4">
+        <v>27410</v>
+      </c>
+      <c r="F14" s="1">
+        <v>169</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="4">
+        <v>26061</v>
+      </c>
+      <c r="F15" s="1">
+        <v>160</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="4">
+        <v>25679</v>
+      </c>
+      <c r="F16" s="1">
+        <v>185</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="4">
+        <v>29653</v>
+      </c>
+      <c r="F17" s="1">
+        <v>190</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="4">
+        <v>25845</v>
+      </c>
+      <c r="F18" s="1">
+        <v>156</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="4">
+        <v>34493</v>
+      </c>
+      <c r="F19" s="1">
+        <v>186</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" s="4">
+        <v>28372</v>
+      </c>
+      <c r="F20" s="1">
+        <v>177</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="2">
+        <v>43831</v>
+      </c>
+      <c r="D24" s="2">
+        <v>43832</v>
+      </c>
+      <c r="E24" s="2">
+        <v>43833</v>
+      </c>
+      <c r="F24" s="2">
+        <v>43834</v>
+      </c>
+      <c r="G24" s="2">
+        <v>43835</v>
+      </c>
+      <c r="H24" s="2">
+        <v>43836</v>
+      </c>
+      <c r="I24" s="2">
+        <v>43837</v>
+      </c>
+      <c r="J24" s="2">
+        <v>43838</v>
+      </c>
+      <c r="K24" s="2">
+        <v>43839</v>
+      </c>
+      <c r="L24" s="2">
+        <v>43840</v>
+      </c>
+      <c r="M24" s="2">
+        <v>43841</v>
+      </c>
+      <c r="N24" s="2">
+        <v>43842</v>
+      </c>
+      <c r="O24" s="2">
+        <v>43843</v>
+      </c>
+      <c r="P24" s="2">
+        <v>43844</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26">
+        <v>87.87</v>
+      </c>
+      <c r="D26" s="3">
+        <v>148.78</v>
+      </c>
+      <c r="E26" s="3">
+        <v>146</v>
+      </c>
+      <c r="F26" s="3">
+        <v>122.82</v>
+      </c>
+      <c r="G26" s="3">
+        <v>59.77</v>
+      </c>
+      <c r="H26" s="3">
+        <v>185.34</v>
+      </c>
+      <c r="I26" s="3">
+        <v>161.47</v>
+      </c>
+      <c r="J26" s="3">
+        <v>102.02</v>
+      </c>
+      <c r="K26" s="3">
+        <v>159.44999999999999</v>
+      </c>
+      <c r="L26" s="3">
+        <v>141.33000000000001</v>
+      </c>
+      <c r="M26" s="3">
+        <v>56.67</v>
+      </c>
+      <c r="N26" s="3">
+        <v>103.83</v>
+      </c>
+      <c r="O26" s="3">
+        <v>153.31</v>
+      </c>
+      <c r="P26" s="3">
+        <v>143.16999999999999</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>56.2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27">
+        <v>135.18</v>
+      </c>
+      <c r="D27" s="3">
+        <v>117.32</v>
+      </c>
+      <c r="E27" s="3">
+        <v>118.39</v>
+      </c>
+      <c r="F27" s="3">
+        <v>134.72999999999999</v>
+      </c>
+      <c r="G27" s="3">
+        <v>70.069999999999993</v>
+      </c>
+      <c r="H27" s="3">
+        <v>90.45</v>
+      </c>
+      <c r="I27" s="3">
+        <v>114.41</v>
+      </c>
+      <c r="J27" s="3">
+        <v>106.34</v>
+      </c>
+      <c r="K27" s="3">
+        <v>146</v>
+      </c>
+      <c r="L27" s="3">
+        <v>118.09</v>
+      </c>
+      <c r="M27" s="3">
+        <v>76.72</v>
+      </c>
+      <c r="N27" s="3">
+        <v>68.98</v>
+      </c>
+      <c r="O27" s="3">
+        <v>118.72</v>
+      </c>
+      <c r="P27" s="3">
+        <v>117.26</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>58.81</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28">
+        <f t="shared" ref="C28:Q28" si="0">SUM(C26:C27)</f>
+        <v>223.05</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>266.10000000000002</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>264.39</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>257.54999999999995</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>129.84</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="0"/>
+        <v>275.79000000000002</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="0"/>
+        <v>275.88</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="0"/>
+        <v>208.36</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="0"/>
+        <v>305.45</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="0"/>
+        <v>259.42</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="0"/>
+        <v>133.38999999999999</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="0"/>
+        <v>172.81</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="0"/>
+        <v>272.02999999999997</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="0"/>
+        <v>260.43</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="0"/>
+        <v>115.01</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA42575C-1408-4827-B59A-7A3D15E02F5F}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>